<commit_message>
Solved Array Problems of DSA Sheet
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,7 +1429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1491,13 +1491,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1509,11 +1545,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1537,9 +1576,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1854,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1886,11 +1937,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="C5" s="4" t="s">
-        <v>465</v>
-      </c>
-    </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
         <v>5</v>
@@ -1898,7 +1944,7 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1909,7 +1955,7 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1920,8 +1966,8 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="C8" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1931,7 +1977,7 @@
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1942,7 +1988,7 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1953,8 +1999,8 @@
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
+      <c r="C11" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1964,8 +2010,8 @@
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
+      <c r="C12" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1975,8 +2021,8 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
+      <c r="C13" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -1986,8 +2032,8 @@
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
+      <c r="C14" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
@@ -1997,7 +2043,7 @@
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2008,8 +2054,8 @@
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
+      <c r="C16" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2030,8 +2076,8 @@
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
+      <c r="C18" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2041,8 +2087,8 @@
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
+      <c r="C19" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2052,8 +2098,8 @@
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
+      <c r="C20" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2063,8 +2109,8 @@
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
+      <c r="C21" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2085,8 +2131,8 @@
       <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
+      <c r="C23" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2096,8 +2142,8 @@
       <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
+      <c r="C24" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2107,7 +2153,7 @@
       <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2118,8 +2164,8 @@
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>4</v>
+      <c r="C26" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Started Search and Sort portions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1891,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2487,8 +2487,8 @@
       <c r="B59" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>4</v>
+      <c r="C59" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2795,8 +2795,8 @@
       <c r="B87" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>4</v>
+      <c r="C87" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="21">
@@ -2806,8 +2806,8 @@
       <c r="B88" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>4</v>
+      <c r="C88" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="21">
@@ -2817,8 +2817,8 @@
       <c r="B89" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>4</v>
+      <c r="C89" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21">
@@ -2861,8 +2861,8 @@
       <c r="B93" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>4</v>
+      <c r="C93" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="21">
@@ -2894,8 +2894,8 @@
       <c r="B96" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>4</v>
+      <c r="C96" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21">
@@ -2905,8 +2905,8 @@
       <c r="B97" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>4</v>
+      <c r="C97" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21">
@@ -2943,8 +2943,8 @@
       <c r="B102" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>4</v>
+      <c r="C102" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2954,8 +2954,8 @@
       <c r="B103" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>4</v>
+      <c r="C103" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -2965,8 +2965,8 @@
       <c r="B104" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>4</v>
+      <c r="C104" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -2976,8 +2976,8 @@
       <c r="B105" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>4</v>
+      <c r="C105" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
@@ -2998,8 +2998,8 @@
       <c r="B107" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>4</v>
+      <c r="C107" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="21">
@@ -3009,8 +3009,8 @@
       <c r="B108" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>4</v>
+      <c r="C108" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="21">
@@ -3020,8 +3020,8 @@
       <c r="B109" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>4</v>
+      <c r="C109" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="21">
@@ -3031,8 +3031,8 @@
       <c r="B110" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="4" t="s">
-        <v>4</v>
+      <c r="C110" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21">
@@ -3042,8 +3042,8 @@
       <c r="B111" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>4</v>
+      <c r="C111" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="21">
@@ -3053,8 +3053,8 @@
       <c r="B112" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="4" t="s">
-        <v>4</v>
+      <c r="C112" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21">
@@ -3064,8 +3064,8 @@
       <c r="B113" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>4</v>
+      <c r="C113" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="21">
@@ -3075,8 +3075,8 @@
       <c r="B114" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="4" t="s">
-        <v>4</v>
+      <c r="C114" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21">
@@ -3086,8 +3086,8 @@
       <c r="B115" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="4" t="s">
-        <v>4</v>
+      <c r="C115" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="21">
@@ -3097,8 +3097,8 @@
       <c r="B116" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>4</v>
+      <c r="C116" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Done some miscellaneous problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="B275" sqref="B275"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3372,8 +3372,8 @@
       <c r="B141" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C141" s="4" t="s">
-        <v>4</v>
+      <c r="C141" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3383,8 +3383,8 @@
       <c r="B142" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C142" s="4" t="s">
-        <v>4</v>
+      <c r="C142" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
@@ -3394,8 +3394,8 @@
       <c r="B143" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C143" s="4" t="s">
-        <v>4</v>
+      <c r="C143" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
@@ -3405,8 +3405,8 @@
       <c r="B144" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C144" s="4" t="s">
-        <v>4</v>
+      <c r="C144" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3416,8 +3416,8 @@
       <c r="B145" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C145" s="4" t="s">
-        <v>4</v>
+      <c r="C145" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -3427,8 +3427,8 @@
       <c r="B146" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C146" s="4" t="s">
-        <v>4</v>
+      <c r="C146" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
@@ -3438,8 +3438,8 @@
       <c r="B147" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C147" s="4" t="s">
-        <v>4</v>
+      <c r="C147" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3449,8 +3449,8 @@
       <c r="B148" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C148" s="4" t="s">
-        <v>4</v>
+      <c r="C148" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">
@@ -3460,8 +3460,8 @@
       <c r="B149" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C149" s="4" t="s">
-        <v>4</v>
+      <c r="C149" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">
@@ -3471,8 +3471,8 @@
       <c r="B150" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C150" s="4" t="s">
-        <v>4</v>
+      <c r="C150" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21">
@@ -3482,8 +3482,8 @@
       <c r="B151" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C151" s="4" t="s">
-        <v>4</v>
+      <c r="C151" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -3493,8 +3493,8 @@
       <c r="B152" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C152" s="4" t="s">
-        <v>4</v>
+      <c r="C152" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">
@@ -3504,8 +3504,8 @@
       <c r="B153" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>4</v>
+      <c r="C153" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21">
@@ -3515,8 +3515,8 @@
       <c r="B154" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C154" s="4" t="s">
-        <v>4</v>
+      <c r="C154" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3526,8 +3526,8 @@
       <c r="B155" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C155" s="4" t="s">
-        <v>4</v>
+      <c r="C155" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21">
@@ -3537,8 +3537,8 @@
       <c r="B156" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C156" s="4" t="s">
-        <v>4</v>
+      <c r="C156" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">
@@ -3548,8 +3548,8 @@
       <c r="B157" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C157" s="4" t="s">
-        <v>4</v>
+      <c r="C157" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21">
@@ -3559,8 +3559,8 @@
       <c r="B158" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C158" s="4" t="s">
-        <v>4</v>
+      <c r="C158" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3570,8 +3570,8 @@
       <c r="B159" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C159" s="4" t="s">
-        <v>4</v>
+      <c r="C159" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">
@@ -3581,8 +3581,8 @@
       <c r="B160" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C160" s="4" t="s">
-        <v>4</v>
+      <c r="C160" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
@@ -3783,8 +3783,8 @@
       <c r="B180" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="4" t="s">
-        <v>4</v>
+      <c r="C180" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3794,8 +3794,8 @@
       <c r="B181" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C181" s="4" t="s">
-        <v>4</v>
+      <c r="C181" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -4788,8 +4788,8 @@
       <c r="B275" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C275" s="4" t="s">
-        <v>4</v>
+      <c r="C275" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Done some Linked List problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1899,7 +1899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3592,8 +3592,8 @@
       <c r="B161" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>4</v>
+      <c r="C161" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">
@@ -3603,8 +3603,8 @@
       <c r="B162" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C162" s="4" t="s">
-        <v>4</v>
+      <c r="C162" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">
@@ -3614,8 +3614,8 @@
       <c r="B163" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C163" s="4" t="s">
-        <v>4</v>
+      <c r="C163" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
@@ -3625,8 +3625,8 @@
       <c r="B164" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C164" s="4" t="s">
-        <v>4</v>
+      <c r="C164" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21">
@@ -3647,8 +3647,8 @@
       <c r="B166" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C166" s="4" t="s">
-        <v>4</v>
+      <c r="C166" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="21">
@@ -3658,8 +3658,8 @@
       <c r="B167" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C167" s="4" t="s">
-        <v>4</v>
+      <c r="C167" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">
@@ -3680,8 +3680,8 @@
       <c r="B169" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C169" s="4" t="s">
-        <v>4</v>
+      <c r="C169" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21">
@@ -3691,8 +3691,8 @@
       <c r="B170" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C170" s="4" t="s">
-        <v>4</v>
+      <c r="C170" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="21">
@@ -3702,8 +3702,8 @@
       <c r="B171" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C171" s="4" t="s">
-        <v>4</v>
+      <c r="C171" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="21">
@@ -3713,8 +3713,8 @@
       <c r="B172" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C172" s="4" t="s">
-        <v>4</v>
+      <c r="C172" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="21">
@@ -3724,8 +3724,8 @@
       <c r="B173" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C173" s="4" t="s">
-        <v>4</v>
+      <c r="C173" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="21">
@@ -3735,9 +3735,7 @@
       <c r="B174" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C174" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C174" s="4"/>
     </row>
     <row r="176" spans="1:3" ht="21">
       <c r="B176" s="7"/>

</xml_diff>

<commit_message>
Started Binary Tree Problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1899,7 +1899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="B164" sqref="B164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B403" sqref="B403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3803,8 +3803,8 @@
       <c r="B182" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C182" s="4" t="s">
-        <v>4</v>
+      <c r="C182" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3814,8 +3814,8 @@
       <c r="B183" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C183" s="4" t="s">
-        <v>4</v>
+      <c r="C183" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3825,8 +3825,8 @@
       <c r="B184" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C184" s="4" t="s">
-        <v>4</v>
+      <c r="C184" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3836,8 +3836,8 @@
       <c r="B185" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C185" s="4" t="s">
-        <v>4</v>
+      <c r="C185" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3847,8 +3847,8 @@
       <c r="B186" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="4" t="s">
-        <v>4</v>
+      <c r="C186" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3858,8 +3858,8 @@
       <c r="B187" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>4</v>
+      <c r="C187" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3869,8 +3869,8 @@
       <c r="B188" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C188" s="4" t="s">
-        <v>4</v>
+      <c r="C188" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3880,8 +3880,8 @@
       <c r="B189" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C189" s="4" t="s">
-        <v>4</v>
+      <c r="C189" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved more Binary Tree Problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1899,7 +1899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B403" sqref="B403"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3891,8 +3891,8 @@
       <c r="B190" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C190" s="4" t="s">
-        <v>4</v>
+      <c r="C190" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3902,8 +3902,8 @@
       <c r="B191" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="4" t="s">
-        <v>4</v>
+      <c r="C191" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -3913,8 +3913,8 @@
       <c r="B192" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="4" t="s">
-        <v>4</v>
+      <c r="C192" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">
@@ -3924,8 +3924,8 @@
       <c r="B193" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>4</v>
+      <c r="C193" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="21">
@@ -3935,8 +3935,8 @@
       <c r="B194" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>4</v>
+      <c r="C194" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="21">
@@ -3946,8 +3946,8 @@
       <c r="B195" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C195" s="4" t="s">
-        <v>4</v>
+      <c r="C195" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="21">
@@ -3968,8 +3968,8 @@
       <c r="B197" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C197" s="4" t="s">
-        <v>4</v>
+      <c r="C197" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="21">
@@ -3979,8 +3979,8 @@
       <c r="B198" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C198" s="4" t="s">
-        <v>4</v>
+      <c r="C198" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="21">
@@ -3990,8 +3990,8 @@
       <c r="B199" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C199" s="4" t="s">
-        <v>4</v>
+      <c r="C199" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="21">
@@ -4001,8 +4001,8 @@
       <c r="B200" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C200" s="4" t="s">
-        <v>4</v>
+      <c r="C200" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved more Binary Search Tree Problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B235" sqref="B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4154,8 +4154,8 @@
       <c r="B215" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>4</v>
+      <c r="C215" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="21">
@@ -4165,8 +4165,8 @@
       <c r="B216" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C216" s="4" t="s">
-        <v>4</v>
+      <c r="C216" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4187,8 +4187,8 @@
       <c r="B218" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C218" s="4" t="s">
-        <v>4</v>
+      <c r="C218" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4198,8 +4198,8 @@
       <c r="B219" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C219" s="4" t="s">
-        <v>4</v>
+      <c r="C219" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="21">
@@ -4209,8 +4209,8 @@
       <c r="B220" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C220" s="4" t="s">
-        <v>4</v>
+      <c r="C220" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="21">
@@ -4220,8 +4220,8 @@
       <c r="B221" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>4</v>
+      <c r="C221" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="21">
@@ -4231,8 +4231,8 @@
       <c r="B222" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>4</v>
+      <c r="C222" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="21">
@@ -4242,8 +4242,8 @@
       <c r="B223" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C223" s="4" t="s">
-        <v>4</v>
+      <c r="C223" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="21">
@@ -4253,8 +4253,8 @@
       <c r="B224" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C224" s="4" t="s">
-        <v>4</v>
+      <c r="C224" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="21">
@@ -4264,8 +4264,8 @@
       <c r="B225" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C225" s="4" t="s">
-        <v>4</v>
+      <c r="C225" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="21">
@@ -4275,8 +4275,8 @@
       <c r="B226" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C226" s="4" t="s">
-        <v>4</v>
+      <c r="C226" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="21">
@@ -4286,8 +4286,8 @@
       <c r="B227" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C227" s="4" t="s">
-        <v>4</v>
+      <c r="C227" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="21">
@@ -4308,8 +4308,8 @@
       <c r="B229" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C229" s="4" t="s">
-        <v>4</v>
+      <c r="C229" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="21">
@@ -4341,8 +4341,8 @@
       <c r="B232" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>4</v>
+      <c r="C232" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="21">
@@ -4352,8 +4352,8 @@
       <c r="B233" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C233" s="4" t="s">
-        <v>4</v>
+      <c r="C233" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="21">
@@ -4374,8 +4374,8 @@
       <c r="B235" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C235" s="4" t="s">
-        <v>4</v>
+      <c r="C235" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">
@@ -4393,8 +4393,8 @@
       <c r="B238" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C238" s="4" t="s">
-        <v>4</v>
+      <c r="C238" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
@@ -5003,8 +5003,8 @@
       <c r="B296" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C296" s="4" t="s">
-        <v>4</v>
+      <c r="C296" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
@@ -7181,246 +7181,246 @@
     <hyperlink ref="B224" r:id="rId204"/>
     <hyperlink ref="B225" r:id="rId205"/>
     <hyperlink ref="B226" r:id="rId206"/>
-    <hyperlink ref="B227" r:id="rId207"/>
-    <hyperlink ref="B228" r:id="rId208"/>
-    <hyperlink ref="B229" r:id="rId209"/>
-    <hyperlink ref="B230" r:id="rId210"/>
-    <hyperlink ref="B231" r:id="rId211"/>
-    <hyperlink ref="B232" r:id="rId212"/>
-    <hyperlink ref="B233" r:id="rId213"/>
-    <hyperlink ref="B234" r:id="rId214"/>
-    <hyperlink ref="B235" r:id="rId215"/>
-    <hyperlink ref="B238" r:id="rId216"/>
-    <hyperlink ref="B239" r:id="rId217"/>
-    <hyperlink ref="B240" r:id="rId218"/>
-    <hyperlink ref="B241" r:id="rId219"/>
-    <hyperlink ref="B242" r:id="rId220"/>
-    <hyperlink ref="B243" r:id="rId221"/>
-    <hyperlink ref="B244" r:id="rId222"/>
-    <hyperlink ref="B245" r:id="rId223"/>
-    <hyperlink ref="B246" r:id="rId224"/>
-    <hyperlink ref="B247" r:id="rId225"/>
-    <hyperlink ref="B248" r:id="rId226"/>
-    <hyperlink ref="B249" r:id="rId227"/>
-    <hyperlink ref="B250" r:id="rId228"/>
-    <hyperlink ref="B251" r:id="rId229"/>
-    <hyperlink ref="B252" r:id="rId230"/>
-    <hyperlink ref="B253" r:id="rId231"/>
-    <hyperlink ref="B254" r:id="rId232"/>
-    <hyperlink ref="B255" r:id="rId233"/>
-    <hyperlink ref="B256" r:id="rId234"/>
-    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId236"/>
-    <hyperlink ref="B259" r:id="rId237"/>
-    <hyperlink ref="B260" r:id="rId238"/>
-    <hyperlink ref="B261" r:id="rId239"/>
-    <hyperlink ref="B262" r:id="rId240"/>
-    <hyperlink ref="B263" r:id="rId241"/>
-    <hyperlink ref="B264" r:id="rId242"/>
-    <hyperlink ref="B265" r:id="rId243"/>
-    <hyperlink ref="B266" r:id="rId244"/>
-    <hyperlink ref="B267" r:id="rId245"/>
-    <hyperlink ref="B268" r:id="rId246"/>
-    <hyperlink ref="B269" r:id="rId247"/>
-    <hyperlink ref="B270" r:id="rId248"/>
-    <hyperlink ref="B271" r:id="rId249"/>
-    <hyperlink ref="B272" r:id="rId250"/>
-    <hyperlink ref="B275" r:id="rId251"/>
-    <hyperlink ref="B276" r:id="rId252"/>
-    <hyperlink ref="B277" r:id="rId253"/>
-    <hyperlink ref="B278" r:id="rId254"/>
-    <hyperlink ref="B279" r:id="rId255"/>
-    <hyperlink ref="B280" r:id="rId256"/>
-    <hyperlink ref="B281" r:id="rId257"/>
-    <hyperlink ref="B282" r:id="rId258"/>
-    <hyperlink ref="B283" r:id="rId259"/>
-    <hyperlink ref="B284" r:id="rId260"/>
-    <hyperlink ref="B285" r:id="rId261"/>
-    <hyperlink ref="B286" r:id="rId262"/>
-    <hyperlink ref="B287" r:id="rId263"/>
-    <hyperlink ref="B288" r:id="rId264"/>
-    <hyperlink ref="B289" r:id="rId265"/>
-    <hyperlink ref="B290" r:id="rId266"/>
-    <hyperlink ref="B291" r:id="rId267"/>
-    <hyperlink ref="B292" r:id="rId268"/>
-    <hyperlink ref="B293" r:id="rId269"/>
-    <hyperlink ref="B296" r:id="rId270"/>
-    <hyperlink ref="B297" r:id="rId271"/>
-    <hyperlink ref="B298" r:id="rId272"/>
-    <hyperlink ref="B299" r:id="rId273"/>
-    <hyperlink ref="B300" r:id="rId274"/>
-    <hyperlink ref="B301" r:id="rId275"/>
-    <hyperlink ref="B302" r:id="rId276"/>
-    <hyperlink ref="B303" r:id="rId277"/>
-    <hyperlink ref="B304" r:id="rId278"/>
-    <hyperlink ref="B305" r:id="rId279"/>
-    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId281"/>
-    <hyperlink ref="B308" r:id="rId282"/>
-    <hyperlink ref="B309" r:id="rId283"/>
-    <hyperlink ref="B310" r:id="rId284"/>
-    <hyperlink ref="B311" r:id="rId285"/>
-    <hyperlink ref="B312" r:id="rId286"/>
-    <hyperlink ref="B313" r:id="rId287"/>
-    <hyperlink ref="B314" r:id="rId288"/>
-    <hyperlink ref="B315" r:id="rId289"/>
-    <hyperlink ref="B316" r:id="rId290"/>
-    <hyperlink ref="B317" r:id="rId291"/>
-    <hyperlink ref="B318" r:id="rId292"/>
-    <hyperlink ref="B319" r:id="rId293"/>
-    <hyperlink ref="B320" r:id="rId294"/>
-    <hyperlink ref="B321" r:id="rId295"/>
-    <hyperlink ref="B322" r:id="rId296"/>
-    <hyperlink ref="B323" r:id="rId297"/>
-    <hyperlink ref="B324" r:id="rId298"/>
-    <hyperlink ref="B325" r:id="rId299"/>
-    <hyperlink ref="B326" r:id="rId300"/>
-    <hyperlink ref="B327" r:id="rId301"/>
-    <hyperlink ref="B328" r:id="rId302"/>
-    <hyperlink ref="B329" r:id="rId303"/>
-    <hyperlink ref="B330" r:id="rId304"/>
-    <hyperlink ref="B331" r:id="rId305"/>
-    <hyperlink ref="B332" r:id="rId306"/>
-    <hyperlink ref="B333" r:id="rId307"/>
-    <hyperlink ref="B336" r:id="rId308"/>
-    <hyperlink ref="B337" r:id="rId309"/>
-    <hyperlink ref="B338" r:id="rId310"/>
-    <hyperlink ref="B339" r:id="rId311"/>
-    <hyperlink ref="B340" r:id="rId312"/>
-    <hyperlink ref="B341" r:id="rId313"/>
-    <hyperlink ref="B342" r:id="rId314"/>
-    <hyperlink ref="B343" r:id="rId315"/>
-    <hyperlink ref="B344" r:id="rId316"/>
-    <hyperlink ref="B345" r:id="rId317"/>
-    <hyperlink ref="B346" r:id="rId318"/>
-    <hyperlink ref="B347" r:id="rId319"/>
-    <hyperlink ref="B348" r:id="rId320"/>
-    <hyperlink ref="B349" r:id="rId321"/>
-    <hyperlink ref="B350" r:id="rId322"/>
-    <hyperlink ref="B351" r:id="rId323"/>
-    <hyperlink ref="B352" r:id="rId324"/>
-    <hyperlink ref="B353" r:id="rId325"/>
-    <hyperlink ref="B357" r:id="rId326"/>
-    <hyperlink ref="B358" r:id="rId327"/>
-    <hyperlink ref="B359" r:id="rId328"/>
-    <hyperlink ref="B360" r:id="rId329"/>
-    <hyperlink ref="B361" r:id="rId330"/>
-    <hyperlink ref="B362" r:id="rId331"/>
-    <hyperlink ref="B363" r:id="rId332"/>
-    <hyperlink ref="B364" r:id="rId333"/>
-    <hyperlink ref="B365" r:id="rId334"/>
-    <hyperlink ref="B366" r:id="rId335"/>
-    <hyperlink ref="B367" r:id="rId336"/>
-    <hyperlink ref="B368" r:id="rId337"/>
-    <hyperlink ref="B369" r:id="rId338"/>
-    <hyperlink ref="B370" r:id="rId339"/>
-    <hyperlink ref="B371" r:id="rId340"/>
-    <hyperlink ref="B372" r:id="rId341"/>
-    <hyperlink ref="B373" r:id="rId342"/>
-    <hyperlink ref="B374" r:id="rId343"/>
-    <hyperlink ref="B375" r:id="rId344"/>
-    <hyperlink ref="B376" r:id="rId345"/>
-    <hyperlink ref="B377" r:id="rId346"/>
-    <hyperlink ref="B378" r:id="rId347"/>
-    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId349"/>
-    <hyperlink ref="B381" r:id="rId350"/>
-    <hyperlink ref="B382" r:id="rId351"/>
-    <hyperlink ref="B383" r:id="rId352"/>
-    <hyperlink ref="B384" r:id="rId353"/>
-    <hyperlink ref="B385" r:id="rId354"/>
-    <hyperlink ref="B386" r:id="rId355"/>
-    <hyperlink ref="B387" r:id="rId356"/>
-    <hyperlink ref="B388" r:id="rId357"/>
-    <hyperlink ref="B389" r:id="rId358"/>
-    <hyperlink ref="B390" r:id="rId359"/>
-    <hyperlink ref="B391" r:id="rId360"/>
-    <hyperlink ref="B392" r:id="rId361"/>
-    <hyperlink ref="B393" r:id="rId362"/>
-    <hyperlink ref="B394" r:id="rId363"/>
-    <hyperlink ref="B396" r:id="rId364"/>
-    <hyperlink ref="B395" r:id="rId365"/>
-    <hyperlink ref="B397" r:id="rId366"/>
-    <hyperlink ref="B398" r:id="rId367"/>
-    <hyperlink ref="B399" r:id="rId368"/>
-    <hyperlink ref="B402" r:id="rId369"/>
-    <hyperlink ref="B403" r:id="rId370"/>
-    <hyperlink ref="B404" r:id="rId371"/>
-    <hyperlink ref="B405" r:id="rId372"/>
-    <hyperlink ref="B406" r:id="rId373"/>
-    <hyperlink ref="B407" r:id="rId374"/>
-    <hyperlink ref="B410" r:id="rId375"/>
-    <hyperlink ref="B411" r:id="rId376"/>
-    <hyperlink ref="B412" r:id="rId377"/>
-    <hyperlink ref="B413" r:id="rId378"/>
-    <hyperlink ref="B414" r:id="rId379"/>
-    <hyperlink ref="B415" r:id="rId380"/>
-    <hyperlink ref="B416" r:id="rId381"/>
-    <hyperlink ref="B417" r:id="rId382"/>
-    <hyperlink ref="B418" r:id="rId383"/>
-    <hyperlink ref="B419" r:id="rId384"/>
-    <hyperlink ref="B420" r:id="rId385"/>
-    <hyperlink ref="B421" r:id="rId386"/>
-    <hyperlink ref="B422" r:id="rId387"/>
-    <hyperlink ref="B423" r:id="rId388"/>
-    <hyperlink ref="B424" r:id="rId389"/>
-    <hyperlink ref="B425" r:id="rId390"/>
-    <hyperlink ref="B426" r:id="rId391"/>
-    <hyperlink ref="B427" r:id="rId392"/>
-    <hyperlink ref="B428" r:id="rId393"/>
-    <hyperlink ref="B429" r:id="rId394"/>
-    <hyperlink ref="B430" r:id="rId395"/>
-    <hyperlink ref="B431" r:id="rId396"/>
-    <hyperlink ref="B432" r:id="rId397"/>
-    <hyperlink ref="B433" r:id="rId398"/>
-    <hyperlink ref="B434" r:id="rId399"/>
-    <hyperlink ref="B435" r:id="rId400"/>
-    <hyperlink ref="B436" r:id="rId401"/>
-    <hyperlink ref="B437" r:id="rId402"/>
-    <hyperlink ref="B438" r:id="rId403"/>
-    <hyperlink ref="B439" r:id="rId404"/>
-    <hyperlink ref="B440" r:id="rId405"/>
-    <hyperlink ref="B441" r:id="rId406"/>
-    <hyperlink ref="B442" r:id="rId407"/>
-    <hyperlink ref="B443" r:id="rId408"/>
-    <hyperlink ref="B444" r:id="rId409"/>
-    <hyperlink ref="B445" r:id="rId410"/>
-    <hyperlink ref="B446" r:id="rId411"/>
-    <hyperlink ref="B447" r:id="rId412"/>
-    <hyperlink ref="B448" r:id="rId413"/>
-    <hyperlink ref="B449" r:id="rId414"/>
-    <hyperlink ref="B451" r:id="rId415"/>
-    <hyperlink ref="B450" r:id="rId416"/>
-    <hyperlink ref="B452" r:id="rId417"/>
-    <hyperlink ref="B453" r:id="rId418"/>
-    <hyperlink ref="B454" r:id="rId419"/>
-    <hyperlink ref="B455" r:id="rId420"/>
-    <hyperlink ref="B456" r:id="rId421"/>
-    <hyperlink ref="B457" r:id="rId422"/>
-    <hyperlink ref="B458" r:id="rId423"/>
-    <hyperlink ref="B459" r:id="rId424"/>
-    <hyperlink ref="B460" r:id="rId425"/>
-    <hyperlink ref="B461" r:id="rId426"/>
-    <hyperlink ref="B462" r:id="rId427"/>
-    <hyperlink ref="B469" r:id="rId428"/>
-    <hyperlink ref="B468" r:id="rId429"/>
-    <hyperlink ref="B467" r:id="rId430"/>
-    <hyperlink ref="B466" r:id="rId431"/>
-    <hyperlink ref="B465" r:id="rId432"/>
-    <hyperlink ref="B464" r:id="rId433"/>
-    <hyperlink ref="B463" r:id="rId434"/>
-    <hyperlink ref="B472" r:id="rId435"/>
-    <hyperlink ref="B473" r:id="rId436"/>
-    <hyperlink ref="B474" r:id="rId437"/>
-    <hyperlink ref="B475" r:id="rId438"/>
-    <hyperlink ref="B476" r:id="rId439"/>
-    <hyperlink ref="B477" r:id="rId440"/>
-    <hyperlink ref="B478" r:id="rId441"/>
-    <hyperlink ref="B481" r:id="rId442"/>
-    <hyperlink ref="B479" r:id="rId443"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId445"/>
-    <hyperlink ref="B2" r:id="rId446"/>
+    <hyperlink ref="B261" r:id="rId207"/>
+    <hyperlink ref="B262" r:id="rId208"/>
+    <hyperlink ref="B263" r:id="rId209"/>
+    <hyperlink ref="B264" r:id="rId210"/>
+    <hyperlink ref="B265" r:id="rId211"/>
+    <hyperlink ref="B266" r:id="rId212"/>
+    <hyperlink ref="B267" r:id="rId213"/>
+    <hyperlink ref="B268" r:id="rId214"/>
+    <hyperlink ref="B269" r:id="rId215"/>
+    <hyperlink ref="B270" r:id="rId216"/>
+    <hyperlink ref="B271" r:id="rId217"/>
+    <hyperlink ref="B272" r:id="rId218"/>
+    <hyperlink ref="B275" r:id="rId219"/>
+    <hyperlink ref="B276" r:id="rId220"/>
+    <hyperlink ref="B277" r:id="rId221"/>
+    <hyperlink ref="B278" r:id="rId222"/>
+    <hyperlink ref="B279" r:id="rId223"/>
+    <hyperlink ref="B280" r:id="rId224"/>
+    <hyperlink ref="B281" r:id="rId225"/>
+    <hyperlink ref="B282" r:id="rId226"/>
+    <hyperlink ref="B283" r:id="rId227"/>
+    <hyperlink ref="B284" r:id="rId228"/>
+    <hyperlink ref="B285" r:id="rId229"/>
+    <hyperlink ref="B286" r:id="rId230"/>
+    <hyperlink ref="B287" r:id="rId231"/>
+    <hyperlink ref="B288" r:id="rId232"/>
+    <hyperlink ref="B289" r:id="rId233"/>
+    <hyperlink ref="B290" r:id="rId234"/>
+    <hyperlink ref="B291" r:id="rId235"/>
+    <hyperlink ref="B292" r:id="rId236"/>
+    <hyperlink ref="B293" r:id="rId237"/>
+    <hyperlink ref="B296" r:id="rId238"/>
+    <hyperlink ref="B297" r:id="rId239"/>
+    <hyperlink ref="B298" r:id="rId240"/>
+    <hyperlink ref="B299" r:id="rId241"/>
+    <hyperlink ref="B300" r:id="rId242"/>
+    <hyperlink ref="B301" r:id="rId243"/>
+    <hyperlink ref="B302" r:id="rId244"/>
+    <hyperlink ref="B303" r:id="rId245"/>
+    <hyperlink ref="B304" r:id="rId246"/>
+    <hyperlink ref="B305" r:id="rId247"/>
+    <hyperlink ref="B306" r:id="rId248" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId249"/>
+    <hyperlink ref="B308" r:id="rId250"/>
+    <hyperlink ref="B309" r:id="rId251"/>
+    <hyperlink ref="B310" r:id="rId252"/>
+    <hyperlink ref="B311" r:id="rId253"/>
+    <hyperlink ref="B312" r:id="rId254"/>
+    <hyperlink ref="B313" r:id="rId255"/>
+    <hyperlink ref="B314" r:id="rId256"/>
+    <hyperlink ref="B315" r:id="rId257"/>
+    <hyperlink ref="B316" r:id="rId258"/>
+    <hyperlink ref="B317" r:id="rId259"/>
+    <hyperlink ref="B318" r:id="rId260"/>
+    <hyperlink ref="B319" r:id="rId261"/>
+    <hyperlink ref="B320" r:id="rId262"/>
+    <hyperlink ref="B321" r:id="rId263"/>
+    <hyperlink ref="B322" r:id="rId264"/>
+    <hyperlink ref="B323" r:id="rId265"/>
+    <hyperlink ref="B324" r:id="rId266"/>
+    <hyperlink ref="B325" r:id="rId267"/>
+    <hyperlink ref="B326" r:id="rId268"/>
+    <hyperlink ref="B327" r:id="rId269"/>
+    <hyperlink ref="B328" r:id="rId270"/>
+    <hyperlink ref="B329" r:id="rId271"/>
+    <hyperlink ref="B330" r:id="rId272"/>
+    <hyperlink ref="B331" r:id="rId273"/>
+    <hyperlink ref="B332" r:id="rId274"/>
+    <hyperlink ref="B333" r:id="rId275"/>
+    <hyperlink ref="B336" r:id="rId276"/>
+    <hyperlink ref="B337" r:id="rId277"/>
+    <hyperlink ref="B338" r:id="rId278"/>
+    <hyperlink ref="B339" r:id="rId279"/>
+    <hyperlink ref="B340" r:id="rId280"/>
+    <hyperlink ref="B341" r:id="rId281"/>
+    <hyperlink ref="B342" r:id="rId282"/>
+    <hyperlink ref="B343" r:id="rId283"/>
+    <hyperlink ref="B344" r:id="rId284"/>
+    <hyperlink ref="B345" r:id="rId285"/>
+    <hyperlink ref="B346" r:id="rId286"/>
+    <hyperlink ref="B347" r:id="rId287"/>
+    <hyperlink ref="B348" r:id="rId288"/>
+    <hyperlink ref="B349" r:id="rId289"/>
+    <hyperlink ref="B350" r:id="rId290"/>
+    <hyperlink ref="B351" r:id="rId291"/>
+    <hyperlink ref="B352" r:id="rId292"/>
+    <hyperlink ref="B353" r:id="rId293"/>
+    <hyperlink ref="B357" r:id="rId294"/>
+    <hyperlink ref="B358" r:id="rId295"/>
+    <hyperlink ref="B359" r:id="rId296"/>
+    <hyperlink ref="B360" r:id="rId297"/>
+    <hyperlink ref="B361" r:id="rId298"/>
+    <hyperlink ref="B362" r:id="rId299"/>
+    <hyperlink ref="B363" r:id="rId300"/>
+    <hyperlink ref="B364" r:id="rId301"/>
+    <hyperlink ref="B365" r:id="rId302"/>
+    <hyperlink ref="B366" r:id="rId303"/>
+    <hyperlink ref="B367" r:id="rId304"/>
+    <hyperlink ref="B368" r:id="rId305"/>
+    <hyperlink ref="B369" r:id="rId306"/>
+    <hyperlink ref="B370" r:id="rId307"/>
+    <hyperlink ref="B371" r:id="rId308"/>
+    <hyperlink ref="B372" r:id="rId309"/>
+    <hyperlink ref="B373" r:id="rId310"/>
+    <hyperlink ref="B374" r:id="rId311"/>
+    <hyperlink ref="B375" r:id="rId312"/>
+    <hyperlink ref="B376" r:id="rId313"/>
+    <hyperlink ref="B377" r:id="rId314"/>
+    <hyperlink ref="B378" r:id="rId315"/>
+    <hyperlink ref="B379" r:id="rId316" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId317"/>
+    <hyperlink ref="B381" r:id="rId318"/>
+    <hyperlink ref="B382" r:id="rId319"/>
+    <hyperlink ref="B383" r:id="rId320"/>
+    <hyperlink ref="B384" r:id="rId321"/>
+    <hyperlink ref="B385" r:id="rId322"/>
+    <hyperlink ref="B386" r:id="rId323"/>
+    <hyperlink ref="B387" r:id="rId324"/>
+    <hyperlink ref="B388" r:id="rId325"/>
+    <hyperlink ref="B389" r:id="rId326"/>
+    <hyperlink ref="B390" r:id="rId327"/>
+    <hyperlink ref="B391" r:id="rId328"/>
+    <hyperlink ref="B392" r:id="rId329"/>
+    <hyperlink ref="B393" r:id="rId330"/>
+    <hyperlink ref="B394" r:id="rId331"/>
+    <hyperlink ref="B396" r:id="rId332"/>
+    <hyperlink ref="B395" r:id="rId333"/>
+    <hyperlink ref="B397" r:id="rId334"/>
+    <hyperlink ref="B398" r:id="rId335"/>
+    <hyperlink ref="B399" r:id="rId336"/>
+    <hyperlink ref="B402" r:id="rId337"/>
+    <hyperlink ref="B403" r:id="rId338"/>
+    <hyperlink ref="B404" r:id="rId339"/>
+    <hyperlink ref="B405" r:id="rId340"/>
+    <hyperlink ref="B406" r:id="rId341"/>
+    <hyperlink ref="B407" r:id="rId342"/>
+    <hyperlink ref="B410" r:id="rId343"/>
+    <hyperlink ref="B411" r:id="rId344"/>
+    <hyperlink ref="B412" r:id="rId345"/>
+    <hyperlink ref="B413" r:id="rId346"/>
+    <hyperlink ref="B414" r:id="rId347"/>
+    <hyperlink ref="B415" r:id="rId348"/>
+    <hyperlink ref="B416" r:id="rId349"/>
+    <hyperlink ref="B417" r:id="rId350"/>
+    <hyperlink ref="B418" r:id="rId351"/>
+    <hyperlink ref="B419" r:id="rId352"/>
+    <hyperlink ref="B420" r:id="rId353"/>
+    <hyperlink ref="B421" r:id="rId354"/>
+    <hyperlink ref="B422" r:id="rId355"/>
+    <hyperlink ref="B423" r:id="rId356"/>
+    <hyperlink ref="B424" r:id="rId357"/>
+    <hyperlink ref="B425" r:id="rId358"/>
+    <hyperlink ref="B426" r:id="rId359"/>
+    <hyperlink ref="B427" r:id="rId360"/>
+    <hyperlink ref="B428" r:id="rId361"/>
+    <hyperlink ref="B429" r:id="rId362"/>
+    <hyperlink ref="B430" r:id="rId363"/>
+    <hyperlink ref="B431" r:id="rId364"/>
+    <hyperlink ref="B432" r:id="rId365"/>
+    <hyperlink ref="B433" r:id="rId366"/>
+    <hyperlink ref="B434" r:id="rId367"/>
+    <hyperlink ref="B435" r:id="rId368"/>
+    <hyperlink ref="B436" r:id="rId369"/>
+    <hyperlink ref="B437" r:id="rId370"/>
+    <hyperlink ref="B438" r:id="rId371"/>
+    <hyperlink ref="B439" r:id="rId372"/>
+    <hyperlink ref="B440" r:id="rId373"/>
+    <hyperlink ref="B441" r:id="rId374"/>
+    <hyperlink ref="B442" r:id="rId375"/>
+    <hyperlink ref="B443" r:id="rId376"/>
+    <hyperlink ref="B444" r:id="rId377"/>
+    <hyperlink ref="B445" r:id="rId378"/>
+    <hyperlink ref="B446" r:id="rId379"/>
+    <hyperlink ref="B447" r:id="rId380"/>
+    <hyperlink ref="B448" r:id="rId381"/>
+    <hyperlink ref="B449" r:id="rId382"/>
+    <hyperlink ref="B451" r:id="rId383"/>
+    <hyperlink ref="B450" r:id="rId384"/>
+    <hyperlink ref="B452" r:id="rId385"/>
+    <hyperlink ref="B453" r:id="rId386"/>
+    <hyperlink ref="B454" r:id="rId387"/>
+    <hyperlink ref="B455" r:id="rId388"/>
+    <hyperlink ref="B456" r:id="rId389"/>
+    <hyperlink ref="B457" r:id="rId390"/>
+    <hyperlink ref="B458" r:id="rId391"/>
+    <hyperlink ref="B459" r:id="rId392"/>
+    <hyperlink ref="B460" r:id="rId393"/>
+    <hyperlink ref="B461" r:id="rId394"/>
+    <hyperlink ref="B462" r:id="rId395"/>
+    <hyperlink ref="B469" r:id="rId396"/>
+    <hyperlink ref="B468" r:id="rId397"/>
+    <hyperlink ref="B467" r:id="rId398"/>
+    <hyperlink ref="B466" r:id="rId399"/>
+    <hyperlink ref="B465" r:id="rId400"/>
+    <hyperlink ref="B464" r:id="rId401"/>
+    <hyperlink ref="B463" r:id="rId402"/>
+    <hyperlink ref="B472" r:id="rId403"/>
+    <hyperlink ref="B473" r:id="rId404"/>
+    <hyperlink ref="B474" r:id="rId405"/>
+    <hyperlink ref="B475" r:id="rId406"/>
+    <hyperlink ref="B476" r:id="rId407"/>
+    <hyperlink ref="B477" r:id="rId408"/>
+    <hyperlink ref="B478" r:id="rId409"/>
+    <hyperlink ref="B481" r:id="rId410"/>
+    <hyperlink ref="B479" r:id="rId411"/>
+    <hyperlink ref="B480" r:id="rId412" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId413"/>
+    <hyperlink ref="B2" r:id="rId414"/>
+    <hyperlink ref="B260" r:id="rId415"/>
+    <hyperlink ref="B259" r:id="rId416"/>
+    <hyperlink ref="B258" r:id="rId417"/>
+    <hyperlink ref="B257" r:id="rId418" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B256" r:id="rId419"/>
+    <hyperlink ref="B255" r:id="rId420"/>
+    <hyperlink ref="B254" r:id="rId421"/>
+    <hyperlink ref="B253" r:id="rId422"/>
+    <hyperlink ref="B252" r:id="rId423"/>
+    <hyperlink ref="B251" r:id="rId424"/>
+    <hyperlink ref="B250" r:id="rId425"/>
+    <hyperlink ref="B249" r:id="rId426"/>
+    <hyperlink ref="B248" r:id="rId427"/>
+    <hyperlink ref="B247" r:id="rId428"/>
+    <hyperlink ref="B246" r:id="rId429"/>
+    <hyperlink ref="B245" r:id="rId430"/>
+    <hyperlink ref="B244" r:id="rId431"/>
+    <hyperlink ref="B243" r:id="rId432"/>
+    <hyperlink ref="B242" r:id="rId433"/>
+    <hyperlink ref="B241" r:id="rId434"/>
+    <hyperlink ref="B240" r:id="rId435"/>
+    <hyperlink ref="B239" r:id="rId436"/>
+    <hyperlink ref="B238" r:id="rId437"/>
+    <hyperlink ref="B235" r:id="rId438"/>
+    <hyperlink ref="B234" r:id="rId439"/>
+    <hyperlink ref="B233" r:id="rId440"/>
+    <hyperlink ref="B232" r:id="rId441"/>
+    <hyperlink ref="B231" r:id="rId442"/>
+    <hyperlink ref="B230" r:id="rId443"/>
+    <hyperlink ref="B229" r:id="rId444"/>
+    <hyperlink ref="B228" r:id="rId445"/>
+    <hyperlink ref="B227" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed Backtracking Problems and started Stack and Queues
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akris\Desktop\Love Babbar DSA Sheet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D79C739B-7DD3-4315-921D-62FC4888C956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1423,7 +1417,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11">
     <font>
       <sz val="12"/>
@@ -1908,18 +1902,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="B286" sqref="B286"/>
+    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="B300" sqref="B300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4971,8 +4965,8 @@
       <c r="B291" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C291" s="4" t="s">
-        <v>4</v>
+      <c r="C291" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="21">
@@ -4993,8 +4987,8 @@
       <c r="B293" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C293" s="4" t="s">
-        <v>4</v>
+      <c r="C293" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="21">
@@ -5023,8 +5017,8 @@
       <c r="B297" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C297" s="4" t="s">
-        <v>4</v>
+      <c r="C297" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">
@@ -5034,8 +5028,8 @@
       <c r="B298" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C298" s="4" t="s">
-        <v>4</v>
+      <c r="C298" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21">
@@ -6984,452 +6978,452 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B35" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B36" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B37" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B38" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B39" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B40" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B41" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B44" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B45" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B46" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B47" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B49" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B50" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B51" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B52" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B53" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B56" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B57" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B58" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B60" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B61" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B62" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B63" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B64" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B65" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B66" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B68" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B69" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B70" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B71" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B72" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B73" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B74" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B75" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B76" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B77" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B78" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B79" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B80" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B81" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B82" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B83" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B84" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B85" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B86" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B87" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B88" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B89" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B90" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B91" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B92" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B93" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B94" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B95" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B96" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B97" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B98" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B101" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B102" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B103" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B104" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B107" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B108" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B109" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B110" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B111" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B113" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B114" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="B115" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="B116" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="B117" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="B118" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="B119" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="B120" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="B121" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B122" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="B123" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B124" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="B125" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B126" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="B127" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B128" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="B129" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B130" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="B131" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B132" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="B133" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="B134" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="B135" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="B136" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="B105" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="B112" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="B139" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="B140" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="B141" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="B142" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="B143" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="B144" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="B145" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="B146" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="B147" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="B148" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="B149" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="B150" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="B151" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="B152" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="B153" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="B154" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="B155" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="B156" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="B157" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="B158" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="B159" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="B160" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="B161" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="B162" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="B163" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="B166" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="B167" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="B168" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="B169" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="B170" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="B171" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="B172" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="B173" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="B174" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="B177" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="B178" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="B179" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="B180" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="B181" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="B182" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="B183" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="B184" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="B185" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="B186" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="B187" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="B188" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="B189" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="B190" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="B191" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="B192" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="B193" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="B194" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="B195" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="B196" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="B198" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="B199" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="B200" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="B201" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="B202" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="B204" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="B205" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="B206" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="B207" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="B208" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="B209" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="B210" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="B211" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="B214" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="B215" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="B216" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="B217" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="B218" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="B219" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="B220" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="B221" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="B222" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="B223" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="B224" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="B225" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="B226" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="B261" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="B262" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="B263" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="B264" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="B265" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="B266" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="B267" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="B268" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="B269" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="B270" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="B271" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="B272" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="B275" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="B276" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="B277" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="B278" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="B279" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="B280" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B281" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="B282" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="B283" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="B284" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="B285" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="B286" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="B287" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="B288" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="B289" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="B290" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="B291" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="B292" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="B293" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="B296" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="B297" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="B298" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="B299" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="B300" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="B301" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="B302" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="B303" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="B304" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="B305" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="B306" r:id="rId248" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="B307" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="B308" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="B309" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="B310" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="B311" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="B312" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="B313" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="B314" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="B315" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="B316" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="B317" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="B318" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="B319" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="B320" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="B321" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="B322" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="B323" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="B324" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="B325" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="B326" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="B327" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="B328" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="B329" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="B330" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="B331" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="B332" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="B333" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="B336" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="B337" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="B338" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="B339" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="B340" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="B341" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="B342" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="B343" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="B344" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="B345" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="B346" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="B347" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="B348" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="B349" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="B350" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="B351" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="B352" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="B353" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="B357" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="B358" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="B359" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="B360" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="B361" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="B362" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="B363" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="B364" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="B365" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="B366" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="B367" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="B368" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="B369" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="B370" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="B371" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="B372" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="B373" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="B374" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="B375" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="B376" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="B377" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="B378" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="B379" r:id="rId316" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="B380" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="B381" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="B382" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="B383" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="B384" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="B385" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="B386" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="B387" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="B388" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="B389" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="B390" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="B391" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="B392" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="B393" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="B394" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="B396" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="B395" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="B397" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="B398" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="B399" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="B402" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="B403" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="B404" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="B405" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="B406" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="B407" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="B410" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="B411" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="B412" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="B413" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="B414" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="B415" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="B416" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="B417" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="B418" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="B419" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="B420" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="B421" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="B422" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="B423" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="B424" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="B425" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="B426" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="B427" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="B428" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="B429" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="B430" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="B431" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="B432" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="B433" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="B434" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="B435" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="B436" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="B437" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="B438" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="B439" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="B440" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="B441" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="B442" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="B443" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="B444" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="B445" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="B446" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="B447" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="B448" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="B449" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="B451" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="B450" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="B452" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="B453" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="B454" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="B455" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="B456" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="B457" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="B458" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="B459" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="B460" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="B461" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="B462" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="B469" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="B468" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="B467" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="B466" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="B465" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="B464" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="B463" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="B472" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="B473" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="B474" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="B475" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="B476" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="B477" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="B478" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="B481" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="B479" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="B480" r:id="rId412" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="B356" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="B2" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="B260" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="B259" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="B258" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="B257" r:id="rId418" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="B256" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="B255" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="B254" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="B253" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="B252" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="B251" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="B250" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="B249" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="B248" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="B247" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="B246" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="B245" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="B244" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="B243" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="B242" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="B241" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="B240" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="B239" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="B238" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="B235" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="B234" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="B233" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="B232" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="B231" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="B230" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="B229" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="B228" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="B227" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="B11" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10"/>
+    <hyperlink ref="B16" r:id="rId11"/>
+    <hyperlink ref="B17" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B19" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B21" r:id="rId16"/>
+    <hyperlink ref="B22" r:id="rId17"/>
+    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B24" r:id="rId19"/>
+    <hyperlink ref="B25" r:id="rId20"/>
+    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B27" r:id="rId22"/>
+    <hyperlink ref="B28" r:id="rId23"/>
+    <hyperlink ref="B29" r:id="rId24"/>
+    <hyperlink ref="B30" r:id="rId25"/>
+    <hyperlink ref="B31" r:id="rId26"/>
+    <hyperlink ref="B32" r:id="rId27"/>
+    <hyperlink ref="B33" r:id="rId28"/>
+    <hyperlink ref="B34" r:id="rId29"/>
+    <hyperlink ref="B35" r:id="rId30"/>
+    <hyperlink ref="B36" r:id="rId31"/>
+    <hyperlink ref="B37" r:id="rId32"/>
+    <hyperlink ref="B38" r:id="rId33"/>
+    <hyperlink ref="B39" r:id="rId34"/>
+    <hyperlink ref="B40" r:id="rId35"/>
+    <hyperlink ref="B41" r:id="rId36"/>
+    <hyperlink ref="B44" r:id="rId37"/>
+    <hyperlink ref="B45" r:id="rId38"/>
+    <hyperlink ref="B46" r:id="rId39"/>
+    <hyperlink ref="B47" r:id="rId40"/>
+    <hyperlink ref="B48" r:id="rId41"/>
+    <hyperlink ref="B49" r:id="rId42"/>
+    <hyperlink ref="B50" r:id="rId43"/>
+    <hyperlink ref="B51" r:id="rId44"/>
+    <hyperlink ref="B52" r:id="rId45"/>
+    <hyperlink ref="B53" r:id="rId46"/>
+    <hyperlink ref="B56" r:id="rId47"/>
+    <hyperlink ref="B57" r:id="rId48"/>
+    <hyperlink ref="B58" r:id="rId49"/>
+    <hyperlink ref="B60" r:id="rId50"/>
+    <hyperlink ref="B61" r:id="rId51"/>
+    <hyperlink ref="B62" r:id="rId52"/>
+    <hyperlink ref="B63" r:id="rId53"/>
+    <hyperlink ref="B64" r:id="rId54"/>
+    <hyperlink ref="B65" r:id="rId55"/>
+    <hyperlink ref="B66" r:id="rId56"/>
+    <hyperlink ref="B67" r:id="rId57"/>
+    <hyperlink ref="B68" r:id="rId58"/>
+    <hyperlink ref="B69" r:id="rId59"/>
+    <hyperlink ref="B70" r:id="rId60"/>
+    <hyperlink ref="B71" r:id="rId61"/>
+    <hyperlink ref="B72" r:id="rId62"/>
+    <hyperlink ref="B73" r:id="rId63"/>
+    <hyperlink ref="B74" r:id="rId64"/>
+    <hyperlink ref="B75" r:id="rId65"/>
+    <hyperlink ref="B76" r:id="rId66"/>
+    <hyperlink ref="B77" r:id="rId67"/>
+    <hyperlink ref="B78" r:id="rId68"/>
+    <hyperlink ref="B79" r:id="rId69"/>
+    <hyperlink ref="B80" r:id="rId70"/>
+    <hyperlink ref="B81" r:id="rId71"/>
+    <hyperlink ref="B82" r:id="rId72"/>
+    <hyperlink ref="B83" r:id="rId73"/>
+    <hyperlink ref="B84" r:id="rId74"/>
+    <hyperlink ref="B85" r:id="rId75"/>
+    <hyperlink ref="B86" r:id="rId76"/>
+    <hyperlink ref="B87" r:id="rId77"/>
+    <hyperlink ref="B88" r:id="rId78"/>
+    <hyperlink ref="B89" r:id="rId79"/>
+    <hyperlink ref="B90" r:id="rId80"/>
+    <hyperlink ref="B91" r:id="rId81"/>
+    <hyperlink ref="B92" r:id="rId82"/>
+    <hyperlink ref="B93" r:id="rId83"/>
+    <hyperlink ref="B94" r:id="rId84"/>
+    <hyperlink ref="B95" r:id="rId85"/>
+    <hyperlink ref="B96" r:id="rId86"/>
+    <hyperlink ref="B97" r:id="rId87"/>
+    <hyperlink ref="B98" r:id="rId88"/>
+    <hyperlink ref="B101" r:id="rId89"/>
+    <hyperlink ref="B102" r:id="rId90"/>
+    <hyperlink ref="B103" r:id="rId91"/>
+    <hyperlink ref="B104" r:id="rId92"/>
+    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="B107" r:id="rId94"/>
+    <hyperlink ref="B108" r:id="rId95"/>
+    <hyperlink ref="B109" r:id="rId96"/>
+    <hyperlink ref="B110" r:id="rId97"/>
+    <hyperlink ref="B111" r:id="rId98"/>
+    <hyperlink ref="B113" r:id="rId99"/>
+    <hyperlink ref="B114" r:id="rId100"/>
+    <hyperlink ref="B115" r:id="rId101"/>
+    <hyperlink ref="B116" r:id="rId102"/>
+    <hyperlink ref="B117" r:id="rId103"/>
+    <hyperlink ref="B118" r:id="rId104"/>
+    <hyperlink ref="B119" r:id="rId105"/>
+    <hyperlink ref="B120" r:id="rId106"/>
+    <hyperlink ref="B121" r:id="rId107"/>
+    <hyperlink ref="B122" r:id="rId108"/>
+    <hyperlink ref="B123" r:id="rId109"/>
+    <hyperlink ref="B124" r:id="rId110"/>
+    <hyperlink ref="B125" r:id="rId111"/>
+    <hyperlink ref="B126" r:id="rId112"/>
+    <hyperlink ref="B127" r:id="rId113"/>
+    <hyperlink ref="B128" r:id="rId114"/>
+    <hyperlink ref="B129" r:id="rId115"/>
+    <hyperlink ref="B130" r:id="rId116"/>
+    <hyperlink ref="B131" r:id="rId117"/>
+    <hyperlink ref="B132" r:id="rId118"/>
+    <hyperlink ref="B133" r:id="rId119"/>
+    <hyperlink ref="B134" r:id="rId120"/>
+    <hyperlink ref="B135" r:id="rId121"/>
+    <hyperlink ref="B136" r:id="rId122"/>
+    <hyperlink ref="B105" r:id="rId123"/>
+    <hyperlink ref="B112" r:id="rId124"/>
+    <hyperlink ref="B139" r:id="rId125"/>
+    <hyperlink ref="B140" r:id="rId126"/>
+    <hyperlink ref="B141" r:id="rId127"/>
+    <hyperlink ref="B142" r:id="rId128"/>
+    <hyperlink ref="B143" r:id="rId129"/>
+    <hyperlink ref="B144" r:id="rId130"/>
+    <hyperlink ref="B145" r:id="rId131"/>
+    <hyperlink ref="B146" r:id="rId132"/>
+    <hyperlink ref="B147" r:id="rId133"/>
+    <hyperlink ref="B148" r:id="rId134"/>
+    <hyperlink ref="B149" r:id="rId135"/>
+    <hyperlink ref="B150" r:id="rId136"/>
+    <hyperlink ref="B151" r:id="rId137"/>
+    <hyperlink ref="B152" r:id="rId138"/>
+    <hyperlink ref="B153" r:id="rId139"/>
+    <hyperlink ref="B154" r:id="rId140"/>
+    <hyperlink ref="B155" r:id="rId141"/>
+    <hyperlink ref="B156" r:id="rId142"/>
+    <hyperlink ref="B157" r:id="rId143"/>
+    <hyperlink ref="B158" r:id="rId144"/>
+    <hyperlink ref="B159" r:id="rId145"/>
+    <hyperlink ref="B160" r:id="rId146"/>
+    <hyperlink ref="B161" r:id="rId147"/>
+    <hyperlink ref="B162" r:id="rId148"/>
+    <hyperlink ref="B163" r:id="rId149"/>
+    <hyperlink ref="B166" r:id="rId150"/>
+    <hyperlink ref="B167" r:id="rId151"/>
+    <hyperlink ref="B168" r:id="rId152"/>
+    <hyperlink ref="B169" r:id="rId153"/>
+    <hyperlink ref="B170" r:id="rId154"/>
+    <hyperlink ref="B171" r:id="rId155"/>
+    <hyperlink ref="B172" r:id="rId156"/>
+    <hyperlink ref="B173" r:id="rId157"/>
+    <hyperlink ref="B174" r:id="rId158"/>
+    <hyperlink ref="B177" r:id="rId159"/>
+    <hyperlink ref="B178" r:id="rId160"/>
+    <hyperlink ref="B179" r:id="rId161"/>
+    <hyperlink ref="B180" r:id="rId162"/>
+    <hyperlink ref="B181" r:id="rId163"/>
+    <hyperlink ref="B182" r:id="rId164"/>
+    <hyperlink ref="B183" r:id="rId165"/>
+    <hyperlink ref="B184" r:id="rId166"/>
+    <hyperlink ref="B185" r:id="rId167"/>
+    <hyperlink ref="B186" r:id="rId168"/>
+    <hyperlink ref="B187" r:id="rId169"/>
+    <hyperlink ref="B188" r:id="rId170"/>
+    <hyperlink ref="B189" r:id="rId171"/>
+    <hyperlink ref="B190" r:id="rId172"/>
+    <hyperlink ref="B191" r:id="rId173"/>
+    <hyperlink ref="B192" r:id="rId174"/>
+    <hyperlink ref="B193" r:id="rId175"/>
+    <hyperlink ref="B194" r:id="rId176"/>
+    <hyperlink ref="B195" r:id="rId177"/>
+    <hyperlink ref="B196" r:id="rId178"/>
+    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B198" r:id="rId180"/>
+    <hyperlink ref="B199" r:id="rId181"/>
+    <hyperlink ref="B200" r:id="rId182"/>
+    <hyperlink ref="B201" r:id="rId183"/>
+    <hyperlink ref="B202" r:id="rId184"/>
+    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B204" r:id="rId186"/>
+    <hyperlink ref="B205" r:id="rId187"/>
+    <hyperlink ref="B206" r:id="rId188"/>
+    <hyperlink ref="B207" r:id="rId189"/>
+    <hyperlink ref="B208" r:id="rId190"/>
+    <hyperlink ref="B209" r:id="rId191"/>
+    <hyperlink ref="B210" r:id="rId192"/>
+    <hyperlink ref="B211" r:id="rId193"/>
+    <hyperlink ref="B214" r:id="rId194"/>
+    <hyperlink ref="B215" r:id="rId195"/>
+    <hyperlink ref="B216" r:id="rId196"/>
+    <hyperlink ref="B217" r:id="rId197"/>
+    <hyperlink ref="B218" r:id="rId198"/>
+    <hyperlink ref="B219" r:id="rId199"/>
+    <hyperlink ref="B220" r:id="rId200"/>
+    <hyperlink ref="B221" r:id="rId201"/>
+    <hyperlink ref="B222" r:id="rId202"/>
+    <hyperlink ref="B223" r:id="rId203"/>
+    <hyperlink ref="B224" r:id="rId204"/>
+    <hyperlink ref="B225" r:id="rId205"/>
+    <hyperlink ref="B226" r:id="rId206"/>
+    <hyperlink ref="B261" r:id="rId207"/>
+    <hyperlink ref="B262" r:id="rId208"/>
+    <hyperlink ref="B263" r:id="rId209"/>
+    <hyperlink ref="B264" r:id="rId210"/>
+    <hyperlink ref="B265" r:id="rId211"/>
+    <hyperlink ref="B266" r:id="rId212"/>
+    <hyperlink ref="B267" r:id="rId213"/>
+    <hyperlink ref="B268" r:id="rId214"/>
+    <hyperlink ref="B269" r:id="rId215"/>
+    <hyperlink ref="B270" r:id="rId216"/>
+    <hyperlink ref="B271" r:id="rId217"/>
+    <hyperlink ref="B272" r:id="rId218"/>
+    <hyperlink ref="B275" r:id="rId219"/>
+    <hyperlink ref="B276" r:id="rId220"/>
+    <hyperlink ref="B277" r:id="rId221"/>
+    <hyperlink ref="B278" r:id="rId222"/>
+    <hyperlink ref="B279" r:id="rId223"/>
+    <hyperlink ref="B280" r:id="rId224"/>
+    <hyperlink ref="B281" r:id="rId225"/>
+    <hyperlink ref="B282" r:id="rId226"/>
+    <hyperlink ref="B283" r:id="rId227"/>
+    <hyperlink ref="B284" r:id="rId228"/>
+    <hyperlink ref="B285" r:id="rId229"/>
+    <hyperlink ref="B286" r:id="rId230"/>
+    <hyperlink ref="B287" r:id="rId231"/>
+    <hyperlink ref="B288" r:id="rId232"/>
+    <hyperlink ref="B289" r:id="rId233"/>
+    <hyperlink ref="B290" r:id="rId234"/>
+    <hyperlink ref="B291" r:id="rId235"/>
+    <hyperlink ref="B292" r:id="rId236"/>
+    <hyperlink ref="B293" r:id="rId237"/>
+    <hyperlink ref="B296" r:id="rId238"/>
+    <hyperlink ref="B297" r:id="rId239"/>
+    <hyperlink ref="B298" r:id="rId240"/>
+    <hyperlink ref="B299" r:id="rId241"/>
+    <hyperlink ref="B300" r:id="rId242"/>
+    <hyperlink ref="B301" r:id="rId243"/>
+    <hyperlink ref="B302" r:id="rId244"/>
+    <hyperlink ref="B303" r:id="rId245"/>
+    <hyperlink ref="B304" r:id="rId246"/>
+    <hyperlink ref="B305" r:id="rId247"/>
+    <hyperlink ref="B306" r:id="rId248" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId249"/>
+    <hyperlink ref="B308" r:id="rId250"/>
+    <hyperlink ref="B309" r:id="rId251"/>
+    <hyperlink ref="B310" r:id="rId252"/>
+    <hyperlink ref="B311" r:id="rId253"/>
+    <hyperlink ref="B312" r:id="rId254"/>
+    <hyperlink ref="B313" r:id="rId255"/>
+    <hyperlink ref="B314" r:id="rId256"/>
+    <hyperlink ref="B315" r:id="rId257"/>
+    <hyperlink ref="B316" r:id="rId258"/>
+    <hyperlink ref="B317" r:id="rId259"/>
+    <hyperlink ref="B318" r:id="rId260"/>
+    <hyperlink ref="B319" r:id="rId261"/>
+    <hyperlink ref="B320" r:id="rId262"/>
+    <hyperlink ref="B321" r:id="rId263"/>
+    <hyperlink ref="B322" r:id="rId264"/>
+    <hyperlink ref="B323" r:id="rId265"/>
+    <hyperlink ref="B324" r:id="rId266"/>
+    <hyperlink ref="B325" r:id="rId267"/>
+    <hyperlink ref="B326" r:id="rId268"/>
+    <hyperlink ref="B327" r:id="rId269"/>
+    <hyperlink ref="B328" r:id="rId270"/>
+    <hyperlink ref="B329" r:id="rId271"/>
+    <hyperlink ref="B330" r:id="rId272"/>
+    <hyperlink ref="B331" r:id="rId273"/>
+    <hyperlink ref="B332" r:id="rId274"/>
+    <hyperlink ref="B333" r:id="rId275"/>
+    <hyperlink ref="B336" r:id="rId276"/>
+    <hyperlink ref="B337" r:id="rId277"/>
+    <hyperlink ref="B338" r:id="rId278"/>
+    <hyperlink ref="B339" r:id="rId279"/>
+    <hyperlink ref="B340" r:id="rId280"/>
+    <hyperlink ref="B341" r:id="rId281"/>
+    <hyperlink ref="B342" r:id="rId282"/>
+    <hyperlink ref="B343" r:id="rId283"/>
+    <hyperlink ref="B344" r:id="rId284"/>
+    <hyperlink ref="B345" r:id="rId285"/>
+    <hyperlink ref="B346" r:id="rId286"/>
+    <hyperlink ref="B347" r:id="rId287"/>
+    <hyperlink ref="B348" r:id="rId288"/>
+    <hyperlink ref="B349" r:id="rId289"/>
+    <hyperlink ref="B350" r:id="rId290"/>
+    <hyperlink ref="B351" r:id="rId291"/>
+    <hyperlink ref="B352" r:id="rId292"/>
+    <hyperlink ref="B353" r:id="rId293"/>
+    <hyperlink ref="B357" r:id="rId294"/>
+    <hyperlink ref="B358" r:id="rId295"/>
+    <hyperlink ref="B359" r:id="rId296"/>
+    <hyperlink ref="B360" r:id="rId297"/>
+    <hyperlink ref="B361" r:id="rId298"/>
+    <hyperlink ref="B362" r:id="rId299"/>
+    <hyperlink ref="B363" r:id="rId300"/>
+    <hyperlink ref="B364" r:id="rId301"/>
+    <hyperlink ref="B365" r:id="rId302"/>
+    <hyperlink ref="B366" r:id="rId303"/>
+    <hyperlink ref="B367" r:id="rId304"/>
+    <hyperlink ref="B368" r:id="rId305"/>
+    <hyperlink ref="B369" r:id="rId306"/>
+    <hyperlink ref="B370" r:id="rId307"/>
+    <hyperlink ref="B371" r:id="rId308"/>
+    <hyperlink ref="B372" r:id="rId309"/>
+    <hyperlink ref="B373" r:id="rId310"/>
+    <hyperlink ref="B374" r:id="rId311"/>
+    <hyperlink ref="B375" r:id="rId312"/>
+    <hyperlink ref="B376" r:id="rId313"/>
+    <hyperlink ref="B377" r:id="rId314"/>
+    <hyperlink ref="B378" r:id="rId315"/>
+    <hyperlink ref="B379" r:id="rId316" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId317"/>
+    <hyperlink ref="B381" r:id="rId318"/>
+    <hyperlink ref="B382" r:id="rId319"/>
+    <hyperlink ref="B383" r:id="rId320"/>
+    <hyperlink ref="B384" r:id="rId321"/>
+    <hyperlink ref="B385" r:id="rId322"/>
+    <hyperlink ref="B386" r:id="rId323"/>
+    <hyperlink ref="B387" r:id="rId324"/>
+    <hyperlink ref="B388" r:id="rId325"/>
+    <hyperlink ref="B389" r:id="rId326"/>
+    <hyperlink ref="B390" r:id="rId327"/>
+    <hyperlink ref="B391" r:id="rId328"/>
+    <hyperlink ref="B392" r:id="rId329"/>
+    <hyperlink ref="B393" r:id="rId330"/>
+    <hyperlink ref="B394" r:id="rId331"/>
+    <hyperlink ref="B396" r:id="rId332"/>
+    <hyperlink ref="B395" r:id="rId333"/>
+    <hyperlink ref="B397" r:id="rId334"/>
+    <hyperlink ref="B398" r:id="rId335"/>
+    <hyperlink ref="B399" r:id="rId336"/>
+    <hyperlink ref="B402" r:id="rId337"/>
+    <hyperlink ref="B403" r:id="rId338"/>
+    <hyperlink ref="B404" r:id="rId339"/>
+    <hyperlink ref="B405" r:id="rId340"/>
+    <hyperlink ref="B406" r:id="rId341"/>
+    <hyperlink ref="B407" r:id="rId342"/>
+    <hyperlink ref="B410" r:id="rId343"/>
+    <hyperlink ref="B411" r:id="rId344"/>
+    <hyperlink ref="B412" r:id="rId345"/>
+    <hyperlink ref="B413" r:id="rId346"/>
+    <hyperlink ref="B414" r:id="rId347"/>
+    <hyperlink ref="B415" r:id="rId348"/>
+    <hyperlink ref="B416" r:id="rId349"/>
+    <hyperlink ref="B417" r:id="rId350"/>
+    <hyperlink ref="B418" r:id="rId351"/>
+    <hyperlink ref="B419" r:id="rId352"/>
+    <hyperlink ref="B420" r:id="rId353"/>
+    <hyperlink ref="B421" r:id="rId354"/>
+    <hyperlink ref="B422" r:id="rId355"/>
+    <hyperlink ref="B423" r:id="rId356"/>
+    <hyperlink ref="B424" r:id="rId357"/>
+    <hyperlink ref="B425" r:id="rId358"/>
+    <hyperlink ref="B426" r:id="rId359"/>
+    <hyperlink ref="B427" r:id="rId360"/>
+    <hyperlink ref="B428" r:id="rId361"/>
+    <hyperlink ref="B429" r:id="rId362"/>
+    <hyperlink ref="B430" r:id="rId363"/>
+    <hyperlink ref="B431" r:id="rId364"/>
+    <hyperlink ref="B432" r:id="rId365"/>
+    <hyperlink ref="B433" r:id="rId366"/>
+    <hyperlink ref="B434" r:id="rId367"/>
+    <hyperlink ref="B435" r:id="rId368"/>
+    <hyperlink ref="B436" r:id="rId369"/>
+    <hyperlink ref="B437" r:id="rId370"/>
+    <hyperlink ref="B438" r:id="rId371"/>
+    <hyperlink ref="B439" r:id="rId372"/>
+    <hyperlink ref="B440" r:id="rId373"/>
+    <hyperlink ref="B441" r:id="rId374"/>
+    <hyperlink ref="B442" r:id="rId375"/>
+    <hyperlink ref="B443" r:id="rId376"/>
+    <hyperlink ref="B444" r:id="rId377"/>
+    <hyperlink ref="B445" r:id="rId378"/>
+    <hyperlink ref="B446" r:id="rId379"/>
+    <hyperlink ref="B447" r:id="rId380"/>
+    <hyperlink ref="B448" r:id="rId381"/>
+    <hyperlink ref="B449" r:id="rId382"/>
+    <hyperlink ref="B451" r:id="rId383"/>
+    <hyperlink ref="B450" r:id="rId384"/>
+    <hyperlink ref="B452" r:id="rId385"/>
+    <hyperlink ref="B453" r:id="rId386"/>
+    <hyperlink ref="B454" r:id="rId387"/>
+    <hyperlink ref="B455" r:id="rId388"/>
+    <hyperlink ref="B456" r:id="rId389"/>
+    <hyperlink ref="B457" r:id="rId390"/>
+    <hyperlink ref="B458" r:id="rId391"/>
+    <hyperlink ref="B459" r:id="rId392"/>
+    <hyperlink ref="B460" r:id="rId393"/>
+    <hyperlink ref="B461" r:id="rId394"/>
+    <hyperlink ref="B462" r:id="rId395"/>
+    <hyperlink ref="B469" r:id="rId396"/>
+    <hyperlink ref="B468" r:id="rId397"/>
+    <hyperlink ref="B467" r:id="rId398"/>
+    <hyperlink ref="B466" r:id="rId399"/>
+    <hyperlink ref="B465" r:id="rId400"/>
+    <hyperlink ref="B464" r:id="rId401"/>
+    <hyperlink ref="B463" r:id="rId402"/>
+    <hyperlink ref="B472" r:id="rId403"/>
+    <hyperlink ref="B473" r:id="rId404"/>
+    <hyperlink ref="B474" r:id="rId405"/>
+    <hyperlink ref="B475" r:id="rId406"/>
+    <hyperlink ref="B476" r:id="rId407"/>
+    <hyperlink ref="B477" r:id="rId408"/>
+    <hyperlink ref="B478" r:id="rId409"/>
+    <hyperlink ref="B481" r:id="rId410"/>
+    <hyperlink ref="B479" r:id="rId411"/>
+    <hyperlink ref="B480" r:id="rId412" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId413"/>
+    <hyperlink ref="B2" r:id="rId414"/>
+    <hyperlink ref="B260" r:id="rId415"/>
+    <hyperlink ref="B259" r:id="rId416"/>
+    <hyperlink ref="B258" r:id="rId417"/>
+    <hyperlink ref="B257" r:id="rId418" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B256" r:id="rId419"/>
+    <hyperlink ref="B255" r:id="rId420"/>
+    <hyperlink ref="B254" r:id="rId421"/>
+    <hyperlink ref="B253" r:id="rId422"/>
+    <hyperlink ref="B252" r:id="rId423"/>
+    <hyperlink ref="B251" r:id="rId424"/>
+    <hyperlink ref="B250" r:id="rId425"/>
+    <hyperlink ref="B249" r:id="rId426"/>
+    <hyperlink ref="B248" r:id="rId427"/>
+    <hyperlink ref="B247" r:id="rId428"/>
+    <hyperlink ref="B246" r:id="rId429"/>
+    <hyperlink ref="B245" r:id="rId430"/>
+    <hyperlink ref="B244" r:id="rId431"/>
+    <hyperlink ref="B243" r:id="rId432"/>
+    <hyperlink ref="B242" r:id="rId433"/>
+    <hyperlink ref="B241" r:id="rId434"/>
+    <hyperlink ref="B240" r:id="rId435"/>
+    <hyperlink ref="B239" r:id="rId436"/>
+    <hyperlink ref="B238" r:id="rId437"/>
+    <hyperlink ref="B235" r:id="rId438"/>
+    <hyperlink ref="B234" r:id="rId439"/>
+    <hyperlink ref="B233" r:id="rId440"/>
+    <hyperlink ref="B232" r:id="rId441"/>
+    <hyperlink ref="B231" r:id="rId442"/>
+    <hyperlink ref="B230" r:id="rId443"/>
+    <hyperlink ref="B229" r:id="rId444"/>
+    <hyperlink ref="B228" r:id="rId445"/>
+    <hyperlink ref="B227" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Solved more Stack and Queue Problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1902,7 +1902,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1912,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
-      <selection activeCell="B300" sqref="B300"/>
+    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5039,8 +5039,8 @@
       <c r="B299" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C299" s="4" t="s">
-        <v>4</v>
+      <c r="C299" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="21">
@@ -5061,8 +5061,8 @@
       <c r="B301" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C301" s="4" t="s">
-        <v>4</v>
+      <c r="C301" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
@@ -5072,8 +5072,8 @@
       <c r="B302" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="C302" s="4" t="s">
-        <v>4</v>
+      <c r="C302" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">
@@ -5083,8 +5083,8 @@
       <c r="B303" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C303" s="4" t="s">
-        <v>4</v>
+      <c r="C303" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="21">
@@ -5094,8 +5094,8 @@
       <c r="B304" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="C304" s="4" t="s">
-        <v>4</v>
+      <c r="C304" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">
@@ -5127,8 +5127,8 @@
       <c r="B307" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C307" s="4" t="s">
-        <v>4</v>
+      <c r="C307" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">
@@ -5138,8 +5138,8 @@
       <c r="B308" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C308" s="4" t="s">
-        <v>4</v>
+      <c r="C308" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">

</xml_diff>